<commit_message>
Moved Styles/Scripts to external files Added Advanced Query Builder
</commit_message>
<xml_diff>
--- a/app/storage/items.xlsx
+++ b/app/storage/items.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1137" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1165" uniqueCount="8">
   <si>
     <t>CMMF</t>
   </si>
@@ -912,11 +912,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E1180"/>
+  <dimension ref="A1:E1208"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1166" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1180" sqref="E1180"/>
+      <pane ySplit="1" topLeftCell="A1181" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C1194" sqref="C1194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -21039,6 +21039,482 @@
         <v>5</v>
       </c>
     </row>
+    <row r="1181" spans="1:5" ht="15.75">
+      <c r="A1181" s="67">
+        <v>7211002075</v>
+      </c>
+      <c r="B1181" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1181" s="11">
+        <v>10.38</v>
+      </c>
+      <c r="D1181" s="16">
+        <v>48</v>
+      </c>
+      <c r="E1181" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1182" spans="1:5" ht="15.75">
+      <c r="A1182" s="67">
+        <v>2100091113</v>
+      </c>
+      <c r="B1182" s="1">
+        <v>6</v>
+      </c>
+      <c r="C1182" s="11">
+        <v>4.1900000000000004</v>
+      </c>
+      <c r="D1182" s="16">
+        <v>42</v>
+      </c>
+      <c r="E1182" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1183" spans="1:5" ht="15.75">
+      <c r="A1183" s="67">
+        <v>8400001008</v>
+      </c>
+      <c r="B1183" s="11">
+        <v>6</v>
+      </c>
+      <c r="C1183" s="11">
+        <v>21.61</v>
+      </c>
+      <c r="D1183" s="16">
+        <v>15</v>
+      </c>
+      <c r="E1183" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1184" spans="1:5" ht="15.75">
+      <c r="A1184" s="67">
+        <v>7211002033</v>
+      </c>
+      <c r="B1184" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1184" s="11">
+        <v>11.91</v>
+      </c>
+      <c r="D1184" s="16">
+        <v>42</v>
+      </c>
+      <c r="E1184" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1185" spans="1:5" ht="15.75">
+      <c r="A1185" s="67">
+        <v>2100056954</v>
+      </c>
+      <c r="B1185" s="1">
+        <v>6</v>
+      </c>
+      <c r="C1185" s="11">
+        <v>8.0399999999999991</v>
+      </c>
+      <c r="D1185" s="16">
+        <v>63</v>
+      </c>
+      <c r="E1185" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1186" spans="1:5" ht="15.75">
+      <c r="A1186" s="67">
+        <v>2100056962</v>
+      </c>
+      <c r="B1186" s="1">
+        <v>6</v>
+      </c>
+      <c r="C1186" s="11">
+        <v>16.82</v>
+      </c>
+      <c r="D1186" s="16">
+        <v>35</v>
+      </c>
+      <c r="E1186" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1187" spans="1:5" ht="15.75">
+      <c r="A1187" s="67">
+        <v>7211002074</v>
+      </c>
+      <c r="B1187" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1187" s="11">
+        <v>10.38</v>
+      </c>
+      <c r="D1187" s="16">
+        <v>48</v>
+      </c>
+      <c r="E1187" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1188" spans="1:5" ht="15.75">
+      <c r="A1188" s="67">
+        <v>7211002083</v>
+      </c>
+      <c r="B1188" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1188" s="11">
+        <v>11.6</v>
+      </c>
+      <c r="D1188" s="16">
+        <v>48</v>
+      </c>
+      <c r="E1188" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1189" spans="1:5" ht="15.75">
+      <c r="A1189" s="67">
+        <v>7211001959</v>
+      </c>
+      <c r="B1189" s="1">
+        <v>2</v>
+      </c>
+      <c r="C1189" s="11">
+        <v>28.66</v>
+      </c>
+      <c r="D1189" s="16">
+        <v>12</v>
+      </c>
+      <c r="E1189" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1190" spans="1:5" ht="15.75">
+      <c r="A1190" s="67">
+        <v>8400001186</v>
+      </c>
+      <c r="B1190" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1190" s="11">
+        <v>29.98</v>
+      </c>
+      <c r="D1190" s="16">
+        <v>10</v>
+      </c>
+      <c r="E1190" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1191" spans="1:5">
+      <c r="A1191" s="71">
+        <v>1500435542</v>
+      </c>
+      <c r="B1191" s="68">
+        <v>1</v>
+      </c>
+      <c r="C1191" s="69">
+        <v>12.6</v>
+      </c>
+      <c r="D1191" s="68">
+        <v>36</v>
+      </c>
+      <c r="E1191" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1192" spans="1:5">
+      <c r="A1192" s="71">
+        <v>2100085505</v>
+      </c>
+      <c r="B1192" s="68">
+        <v>2</v>
+      </c>
+      <c r="C1192" s="69">
+        <v>9.9209999999999994</v>
+      </c>
+      <c r="D1192" s="68">
+        <v>32</v>
+      </c>
+      <c r="E1192" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1193" spans="1:5">
+      <c r="A1193" s="71">
+        <v>2100089398</v>
+      </c>
+      <c r="B1193" s="68">
+        <v>1</v>
+      </c>
+      <c r="C1193" s="69">
+        <v>18.187999999999999</v>
+      </c>
+      <c r="D1193" s="68">
+        <v>40</v>
+      </c>
+      <c r="E1193" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1194" spans="1:5">
+      <c r="A1194" s="71">
+        <v>8400000029</v>
+      </c>
+      <c r="B1194" s="68">
+        <v>2</v>
+      </c>
+      <c r="C1194" s="69">
+        <v>9.3919999999999995</v>
+      </c>
+      <c r="D1194" s="68">
+        <v>32</v>
+      </c>
+      <c r="E1194" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1195" spans="1:5">
+      <c r="A1195" s="71">
+        <v>8400000255</v>
+      </c>
+      <c r="B1195" s="68">
+        <v>1</v>
+      </c>
+      <c r="C1195" s="69">
+        <v>54.5</v>
+      </c>
+      <c r="D1195" s="68">
+        <v>8</v>
+      </c>
+      <c r="E1195" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1196" spans="1:5">
+      <c r="A1196" s="71">
+        <v>8701004425</v>
+      </c>
+      <c r="B1196" s="68">
+        <v>1</v>
+      </c>
+      <c r="C1196" s="69">
+        <v>3.2850000000000001</v>
+      </c>
+      <c r="D1196" s="68">
+        <v>136</v>
+      </c>
+      <c r="E1196" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1197" spans="1:5">
+      <c r="A1197" s="71">
+        <v>8700800417</v>
+      </c>
+      <c r="B1197" s="68">
+        <v>1</v>
+      </c>
+      <c r="C1197" s="69">
+        <v>5.9969999999999999</v>
+      </c>
+      <c r="D1197" s="68">
+        <v>72</v>
+      </c>
+      <c r="E1197" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1198" spans="1:5">
+      <c r="A1198" s="71">
+        <v>8701004136</v>
+      </c>
+      <c r="B1198" s="68">
+        <v>1</v>
+      </c>
+      <c r="C1198" s="69">
+        <v>6.6139999999999999</v>
+      </c>
+      <c r="D1198" s="68">
+        <v>60</v>
+      </c>
+      <c r="E1198" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1199" spans="1:5">
+      <c r="A1199" s="71">
+        <v>8701004429</v>
+      </c>
+      <c r="B1199" s="68">
+        <v>4</v>
+      </c>
+      <c r="C1199" s="69">
+        <v>11.75</v>
+      </c>
+      <c r="D1199" s="68">
+        <v>49</v>
+      </c>
+      <c r="E1199" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1200" spans="1:5">
+      <c r="A1200" s="71">
+        <v>8701005157</v>
+      </c>
+      <c r="B1200" s="68">
+        <v>6</v>
+      </c>
+      <c r="C1200" s="69">
+        <v>4.2329999999999997</v>
+      </c>
+      <c r="D1200" s="68">
+        <v>216</v>
+      </c>
+      <c r="E1200" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1201" spans="1:5" ht="15.75">
+      <c r="A1201" s="67">
+        <v>2100087475</v>
+      </c>
+      <c r="B1201" s="40">
+        <v>2</v>
+      </c>
+      <c r="C1201" s="11">
+        <v>6.83</v>
+      </c>
+      <c r="D1201" s="16">
+        <v>40</v>
+      </c>
+      <c r="E1201" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1202" spans="1:5" ht="15.75">
+      <c r="A1202" s="67">
+        <v>2100087482</v>
+      </c>
+      <c r="B1202" s="70">
+        <v>2</v>
+      </c>
+      <c r="C1202" s="11">
+        <v>11.24</v>
+      </c>
+      <c r="D1202" s="16">
+        <v>30</v>
+      </c>
+      <c r="E1202" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1203" spans="1:5" ht="15.75">
+      <c r="A1203" s="67">
+        <v>2100088756</v>
+      </c>
+      <c r="B1203" s="11">
+        <v>1</v>
+      </c>
+      <c r="C1203" s="11">
+        <v>14.551</v>
+      </c>
+      <c r="D1203" s="16">
+        <v>36</v>
+      </c>
+      <c r="E1203" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1204" spans="1:5">
+      <c r="A1204" s="49">
+        <v>2100088763</v>
+      </c>
+      <c r="B1204" s="11">
+        <v>1</v>
+      </c>
+      <c r="C1204" s="11">
+        <v>16.975999999999999</v>
+      </c>
+      <c r="D1204" s="16">
+        <v>35</v>
+      </c>
+      <c r="E1204" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1205" spans="1:5">
+      <c r="A1205" s="49">
+        <v>2100089060</v>
+      </c>
+      <c r="B1205" s="11">
+        <v>1</v>
+      </c>
+      <c r="C1205" s="11">
+        <v>17.55</v>
+      </c>
+      <c r="D1205" s="16">
+        <v>35</v>
+      </c>
+      <c r="E1205" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1206" spans="1:5">
+      <c r="A1206" s="49">
+        <v>2100089678</v>
+      </c>
+      <c r="B1206" s="11">
+        <v>1</v>
+      </c>
+      <c r="C1206" s="11">
+        <v>19.620999999999999</v>
+      </c>
+      <c r="D1206" s="16">
+        <v>30</v>
+      </c>
+      <c r="E1206" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1207" spans="1:5">
+      <c r="A1207" s="49">
+        <v>2100089685</v>
+      </c>
+      <c r="B1207" s="11">
+        <v>1</v>
+      </c>
+      <c r="C1207" s="11">
+        <v>20.8</v>
+      </c>
+      <c r="D1207" s="16">
+        <v>12</v>
+      </c>
+      <c r="E1207" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1208" spans="1:5">
+      <c r="A1208" s="49">
+        <v>2100089950</v>
+      </c>
+      <c r="B1208" s="11">
+        <v>1</v>
+      </c>
+      <c r="C1208" s="11">
+        <v>19.620999999999999</v>
+      </c>
+      <c r="D1208" s="16">
+        <v>30</v>
+      </c>
+      <c r="E1208" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:E947">
     <sortState ref="A2:E887">
@@ -21048,12 +21524,12 @@
   <sortState ref="A2:F811">
     <sortCondition descending="1" ref="A1"/>
   </sortState>
-  <conditionalFormatting sqref="A570:A583 A588:A605 A491:A556 A1:A448 A607:A792 A795 A797:A807 A811:A871 A873:A901 A904:A948 A950:A954 A960:A968 A970:A978 A982:A986 A990 A992:A994 A1001:A1006 A1008:A1020 A1022:A1031 A1039:A1044 A1048 A1051 A1065:A1070 A1072:A1075 A1084:A1086 A1089:A1097 A1107:A1114 A1117:A1135 A1157:A1163 A1166:A1170 A1173:A1179 A1181:A1048576">
+  <conditionalFormatting sqref="A570:A583 A588:A605 A491:A556 A1:A448 A607:A792 A795 A797:A807 A811:A871 A873:A901 A904:A948 A950:A954 A960:A968 A970:A978 A982:A986 A990 A992:A994 A1001:A1006 A1008:A1020 A1022:A1031 A1039:A1044 A1048 A1051 A1065:A1070 A1072:A1075 A1084:A1086 A1089:A1097 A1107:A1114 A1117:A1135 A1157:A1163 A1166:A1170 A1173:A1179 A1191:A1200 A1204:A1048576">
     <cfRule type="duplicateValues" dxfId="21" priority="80"/>
     <cfRule type="duplicateValues" dxfId="20" priority="81"/>
     <cfRule type="duplicateValues" dxfId="19" priority="82"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A588:A605 A1:A556 A570:A583 A607:A792 A795 A797:A807 A811:A871 A873:A901 A904:A948 A950:A954 A960:A968 A970:A978 A982:A986 A990 A992:A994 A1001:A1006 A1008:A1020 A1022:A1031 A1039:A1044 A1048 A1051 A1065:A1070 A1072:A1075 A1084:A1086 A1089:A1097 A1107:A1114 A1117:A1135 A1157:A1163 A1166:A1170 A1173:A1179 A1181:A1048576">
+  <conditionalFormatting sqref="A588:A605 A1:A556 A570:A583 A607:A792 A795 A797:A807 A811:A871 A873:A901 A904:A948 A950:A954 A960:A968 A970:A978 A982:A986 A990 A992:A994 A1001:A1006 A1008:A1020 A1022:A1031 A1039:A1044 A1048 A1051 A1065:A1070 A1072:A1075 A1084:A1086 A1089:A1097 A1107:A1114 A1117:A1135 A1157:A1163 A1166:A1170 A1173:A1179 A1191:A1200 A1204:A1048576">
     <cfRule type="duplicateValues" dxfId="18" priority="99"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A165:A178 A147:A163 A1:A145">
@@ -21086,7 +21562,7 @@
   <conditionalFormatting sqref="A856:A869 A819:A842">
     <cfRule type="duplicateValues" dxfId="4" priority="1168"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A873:A901 A1:A871 A904:A948 A950:A954 A960:A968 A970:A978 A982:A986 A990 A992:A994 A1001:A1006 A1008:A1020 A1022:A1031 A1039:A1044 A1048 A1051 A1065:A1070 A1072:A1075 A1084:A1086 A1089:A1097 A1107:A1114 A1117:A1135 A1157:A1163 A1166:A1170 A1173:A1179 A1181:A1048576">
+  <conditionalFormatting sqref="A873:A901 A1:A871 A904:A948 A950:A954 A960:A968 A970:A978 A982:A986 A990 A992:A994 A1001:A1006 A1008:A1020 A1022:A1031 A1039:A1044 A1048 A1051 A1065:A1070 A1072:A1075 A1084:A1086 A1089:A1097 A1107:A1114 A1117:A1135 A1157:A1163 A1166:A1170 A1173:A1179 A1191:A1200 A1204:A1048576">
     <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A217:A241 A209">

</xml_diff>